<commit_message>
Excel datos umd pc
</commit_message>
<xml_diff>
--- a/src/Texto/Graficas algoritmos ordenamiento.xlsx
+++ b/src/Texto/Graficas algoritmos ordenamiento.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Things VLGG\UMD\2019ne\Ing sistemas 2019-2\20192\Diseno Algoritmos\Corte 1\Corte1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BOG-A307-E-010\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129C55D9-370C-4F18-8C6E-D50E12A0F1DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{AAF1C5B0-A4B8-4E87-BBB4-C2FC816DA2E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -65,11 +64,41 @@
   <si>
     <t>cien mil</t>
   </si>
+  <si>
+    <t>Cinco mil</t>
+  </si>
+  <si>
+    <t>Diez mil</t>
+  </si>
+  <si>
+    <t>25 mil</t>
+  </si>
+  <si>
+    <t>50 mil</t>
+  </si>
+  <si>
+    <t>75 mil</t>
+  </si>
+  <si>
+    <t>Cien mil</t>
+  </si>
+  <si>
+    <t>Mil</t>
+  </si>
+  <si>
+    <t>Bubble</t>
+  </si>
+  <si>
+    <t>Quick</t>
+  </si>
+  <si>
+    <t>Merge</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -99,9 +128,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -156,6 +186,32 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO"/>
+              <a:t>Personal</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -181,7 +237,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -520,7 +576,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="646181224"/>
@@ -579,7 +635,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="645944640"/>
@@ -596,6 +652,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -621,7 +678,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -652,7 +709,560 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO"/>
+              <a:t>Umd</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-CO" baseline="0"/>
+              <a:t> pc</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$E$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bubble</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$F$32:$M$32</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Mil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cinco mil</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Diez mil</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25 mil</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50 mil</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75 mil</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Cien mil</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$F$33:$M$33</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>43751</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39154</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1389382</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9890081</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40443317</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88981014</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>156658136</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3A85-42DB-A8A1-272A76DE74A0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$E$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quick</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$F$32:$M$32</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Mil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cinco mil</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Diez mil</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25 mil</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50 mil</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75 mil</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Cien mil</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$F$34:$M$34</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>45746</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16805</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11084</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28931</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8129</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9282</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>122297</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3A85-42DB-A8A1-272A76DE74A0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$E$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Merge</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$F$32:$M$32</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Mil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cinco mil</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Diez mil</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25 mil</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50 mil</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75 mil</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Cien mil</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$F$35:$M$35</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>18728</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>184999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>645114</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4240071</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5569317</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20179699</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27681576</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3A85-42DB-A8A1-272A76DE74A0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1444498368"/>
+        <c:axId val="1444493792"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1444498368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1444493792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1444493792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1444498368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -703,7 +1313,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1257,21 +2423,51 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>389283</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>130036</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>389283</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>15736</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67700D2D-87AA-4659-83FB-16025C66250A}" name="Tabla1" displayName="Tabla1" ref="D3:K6" totalsRowShown="0">
-  <autoFilter ref="D3:K6" xr:uid="{D0493344-D369-4CAC-894F-3885925D9389}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="D3:K6" totalsRowShown="0">
+  <autoFilter ref="D3:K6"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{19DF527A-F28A-49FD-896C-05A5DFA98A78}" name="Algoritmo"/>
-    <tableColumn id="2" xr3:uid="{023414CF-5730-47A0-B1E5-DF1CEA6C406E}" name="mil" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{0A49F987-6CFE-4BC3-A5D7-0CE8491D0FBD}" name="cinco mil" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{13256612-BEF2-4688-AA3E-8D516B838378}" name="diez mil" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{B30C9F61-4F0C-4EA5-A506-AD891D075561}" name="venticinco" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{77AFFEEE-0A9D-425E-A064-D1E87696BF54}" name="cincuenta" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{A301FF24-E524-4AAD-B68F-65F886D0764C}" name="setentaycinco" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{FBD039CD-86E0-4D87-9308-21123D160859}" name="cien mil" dataDxfId="0"/>
+    <tableColumn id="1" name="Algoritmo"/>
+    <tableColumn id="2" name="mil" dataDxfId="6"/>
+    <tableColumn id="3" name="cinco mil" dataDxfId="5"/>
+    <tableColumn id="4" name="diez mil" dataDxfId="4"/>
+    <tableColumn id="5" name="venticinco" dataDxfId="3"/>
+    <tableColumn id="6" name="cincuenta" dataDxfId="2"/>
+    <tableColumn id="7" name="setentaycinco" dataDxfId="1"/>
+    <tableColumn id="8" name="cien mil" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1573,11 +2769,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{031D4ABA-0578-4D77-BC15-D600710F5BD5}">
-  <dimension ref="D3:K6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D3:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,6 +2783,8 @@
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
     <col min="10" max="10" width="20.140625" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:11" x14ac:dyDescent="0.25">
@@ -1691,6 +2889,125 @@
       </c>
       <c r="K6" s="1">
         <v>28460.17656</v>
+      </c>
+    </row>
+    <row r="28" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="M28" s="2">
+        <v>4648721907</v>
+      </c>
+    </row>
+    <row r="29" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="M29" s="2">
+        <v>1578318</v>
+      </c>
+    </row>
+    <row r="30" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="M30" s="2">
+        <v>1549573969</v>
+      </c>
+    </row>
+    <row r="32" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" t="s">
+        <v>15</v>
+      </c>
+      <c r="L32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="2">
+        <v>43751</v>
+      </c>
+      <c r="G33" s="2">
+        <v>39154</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1389382</v>
+      </c>
+      <c r="I33" s="2">
+        <v>9890081</v>
+      </c>
+      <c r="J33" s="2">
+        <v>40443317</v>
+      </c>
+      <c r="K33" s="2">
+        <v>88981014</v>
+      </c>
+      <c r="L33" s="2">
+        <v>156658136</v>
+      </c>
+    </row>
+    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="2">
+        <v>45746</v>
+      </c>
+      <c r="G34" s="2">
+        <v>16805</v>
+      </c>
+      <c r="H34" s="2">
+        <v>11084</v>
+      </c>
+      <c r="I34" s="2">
+        <v>28931</v>
+      </c>
+      <c r="J34" s="2">
+        <v>8129</v>
+      </c>
+      <c r="K34" s="2">
+        <v>9282</v>
+      </c>
+      <c r="L34" s="2">
+        <v>122297</v>
+      </c>
+    </row>
+    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="2">
+        <v>18728</v>
+      </c>
+      <c r="G35" s="2">
+        <v>184999</v>
+      </c>
+      <c r="H35" s="2">
+        <v>645114</v>
+      </c>
+      <c r="I35" s="2">
+        <v>4240071</v>
+      </c>
+      <c r="J35" s="2">
+        <v>5569317</v>
+      </c>
+      <c r="K35" s="2">
+        <v>20179699</v>
+      </c>
+      <c r="L35" s="2">
+        <v>27681576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Menu scanner y metodo unico para crear archivo.
</commit_message>
<xml_diff>
--- a/src/Texto/Graficas algoritmos ordenamiento.xlsx
+++ b/src/Texto/Graficas algoritmos ordenamiento.xlsx
@@ -1,36 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BOG-A307-E-010\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Documents\NetBeansProjects\AlgorithmDesign\src\Texto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C0525B-7345-47EA-B229-D31F8EEDDEDB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Algoritmo</t>
   </si>
@@ -94,11 +91,20 @@
   <si>
     <t>Merge</t>
   </si>
+  <si>
+    <t>2gb ram</t>
+  </si>
+  <si>
+    <t>4gb ram</t>
+  </si>
+  <si>
+    <t>Millon</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -136,7 +142,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -206,12 +236,16 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-CO"/>
-              <a:t>Personal</a:t>
+              <a:t>Velocidad</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="es-CO" baseline="0"/>
+              <a:t> metodos</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -237,7 +271,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -576,7 +610,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="646181224"/>
@@ -635,7 +669,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="645944640"/>
@@ -652,7 +686,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -678,7 +711,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -709,7 +742,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -765,7 +798,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -791,7 +823,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1130,7 +1162,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1444493792"/>
@@ -1189,7 +1221,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CO"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1444498368"/>
@@ -1206,7 +1238,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1232,7 +1263,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CO"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1262,7 +1293,1978 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CO"/>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Velocidad Metodos</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bubblesort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Hoja2!$D$4:$K$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Hoja2!$D$4:$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>mil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cinco mil</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>diez mil</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>venticinco</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cincuenta</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>setentaycinco</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cien mil</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Hoja2!$D$5:$K$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Hoja2!$D$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>36.620809999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>665.260401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>662.50023299999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4250.2130239999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11476.963006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25528.633629</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45097.424034999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3B07-4630-8F95-E7F9D27AE008}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quicksort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Hoja2!$D$4:$K$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Hoja2!$D$4:$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>mil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cinco mil</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>diez mil</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>venticinco</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cincuenta</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>setentaycinco</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cien mil</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Hoja2!$D$6:$K$6</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Hoja2!$D$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15.594155000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.312487000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.802686</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.193071</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.942261999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.030825</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38.522472999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3B07-4630-8F95-E7F9D27AE008}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$C$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mergesort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Hoja2!$D$4:$K$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Hoja2!$D$4:$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>mil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cinco mil</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>diez mil</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>venticinco</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cincuenta</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>setentaycinco</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cien mil</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Hoja2!$D$7:$K$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Hoja2!$D$7:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>14.729879</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>441.14876900000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1619.73973</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2488.3524710000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6175.4351999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13254.281147</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24521.592473000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3B07-4630-8F95-E7F9D27AE008}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="292880656"/>
+        <c:axId val="292877376"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="292880656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="292877376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="292877376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="292880656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bubblesort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja2!$D$4:$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>mil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cinco mil</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>diez mil</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>venticinco</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cincuenta</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>setentaycinco</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cien mil</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$D$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>36.620809999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>665.260401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>662.50023299999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4250.2130239999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11476.963006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25528.633629</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45097.424034999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-40F7-4336-9432-D96DAA7CDB4F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="197566424"/>
+        <c:axId val="197566096"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="197566424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="197566096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="197566096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="197566424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$C$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quicksort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja2!$D$4:$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>mil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cinco mil</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>diez mil</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>venticinco</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cincuenta</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>setentaycinco</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cien mil</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$D$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>15.594155000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.312487000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.802686</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.193071</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.942261999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.030825</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38.522472999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-07B1-4CB6-8093-7695056594CB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="195291256"/>
+        <c:axId val="195291584"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja2!$C$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Bubblesort</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja2!$D$4:$J$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>mil</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>cinco mil</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>diez mil</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>venticinco</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>cincuenta</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>setentaycinco</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>cien mil</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja2!$D$5:$J$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>36.620809999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>665.260401</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>662.50023299999998</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4250.2130239999997</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>11476.963006</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>25528.633629</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>45097.424034999996</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-07B1-4CB6-8093-7695056594CB}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="195291256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="195291584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="195291584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="195291256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja2!$C$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mergesort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja2!$D$4:$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>mil</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cinco mil</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>diez mil</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>venticinco</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cincuenta</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>setentaycinco</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cien mil</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja2!$D$7:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>14.729879</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>441.14876900000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1619.73973</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2488.3524710000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6175.4351999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13254.281147</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24521.592473000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-39D4-44B6-A997-91C861730BAA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="272189296"/>
+        <c:axId val="272189624"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja2!$C$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Bubblesort</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja2!$D$4:$J$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>mil</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>cinco mil</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>diez mil</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>venticinco</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>cincuenta</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>setentaycinco</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>cien mil</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja2!$D$5:$J$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>36.620809999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>665.260401</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>662.50023299999998</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>4250.2130239999997</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>11476.963006</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>25528.633629</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>45097.424034999996</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-39D4-44B6-A997-91C861730BAA}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja2!$C$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Quicksort</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja2!$D$4:$J$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>mil</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>cinco mil</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>diez mil</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>venticinco</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>cincuenta</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>setentaycinco</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>cien mil</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Hoja2!$D$6:$J$6</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="7"/>
+                      <c:pt idx="0">
+                        <c:v>15.594155000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>14.312487000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>3.802686</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>10.193071</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>18.942261999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>29.030825</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>38.522472999999998</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-39D4-44B6-A997-91C861730BAA}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="272189296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="272189624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="272189624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="272189296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1353,6 +3355,166 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1870,6 +4032,2070 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2405,7 +6631,7 @@
         <xdr:cNvPr id="15" name="Gráfico 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05F8C883-C415-4E22-8BAA-1D44264782B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2438,7 +6664,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2456,18 +6688,185 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01AD24F2-D419-4FB4-B6A4-351FEC32B418}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59D8F240-7206-4F38-BA0E-61A4BA8A3C31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>666749</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA58BDB6-A42C-47BB-8DE7-6213028C18C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89A3CAF8-3D26-4E70-9F1A-8D37F2EDFF91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="D3:K6" totalsRowShown="0">
-  <autoFilter ref="D3:K6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="D3:K6" totalsRowShown="0">
+  <autoFilter ref="D3:K6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Algoritmo"/>
-    <tableColumn id="2" name="mil" dataDxfId="6"/>
-    <tableColumn id="3" name="cinco mil" dataDxfId="5"/>
-    <tableColumn id="4" name="diez mil" dataDxfId="4"/>
-    <tableColumn id="5" name="venticinco" dataDxfId="3"/>
-    <tableColumn id="6" name="cincuenta" dataDxfId="2"/>
-    <tableColumn id="7" name="setentaycinco" dataDxfId="1"/>
-    <tableColumn id="8" name="cien mil" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Algoritmo"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="mil" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="cinco mil" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="diez mil" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="venticinco" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="cincuenta" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="setentaycinco" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="cien mil" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{328B6BA8-37D8-40EF-93E4-834123B1899F}" name="Tabla13" displayName="Tabla13" ref="C4:K7" totalsRowShown="0">
+  <autoFilter ref="C4:K7" xr:uid="{C357B706-C1BC-485C-8036-AD7DC8CE8F69}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{9FF54AA9-4234-43A1-B03D-E7F7CBBB9DAD}" name="Algoritmo"/>
+    <tableColumn id="2" xr3:uid="{B9FC5589-66E1-490A-8C1B-F94FE7EA9482}" name="mil" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{B053714C-E62F-4DD1-B1F3-AE69799EA926}" name="cinco mil" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{9E2E7259-675C-43E2-9805-DB1ABE685ABA}" name="diez mil" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{96D7ED34-18FE-484E-B2B1-3035A55206D9}" name="venticinco" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{3DDD6769-8CCF-4F15-ADB5-09A3BE1A2F7F}" name="cincuenta" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{2C0337DB-46FF-49D2-A1AB-B3B03D775E5A}" name="setentaycinco" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{57D92BC4-5E92-4BC7-813C-CCED75DBB9DC}" name="cien mil" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{AD0113A1-304F-489F-8D14-95D4BEE49421}" name="Millon" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2769,11 +7168,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:M35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="D1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2787,6 +7186,11 @@
     <col min="13" max="13" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="3" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>0</v>
@@ -3018,4 +7422,158 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C7329F0-E614-4B72-9BE9-70C6B0ADCEDA}">
+  <dimension ref="C2:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>36.620809999999999</v>
+      </c>
+      <c r="E5">
+        <v>665.260401</v>
+      </c>
+      <c r="F5">
+        <v>662.50023299999998</v>
+      </c>
+      <c r="G5">
+        <v>4250.2130239999997</v>
+      </c>
+      <c r="H5">
+        <v>11476.963006</v>
+      </c>
+      <c r="I5">
+        <v>25528.633629</v>
+      </c>
+      <c r="J5">
+        <v>45097.424034999996</v>
+      </c>
+      <c r="K5" s="1">
+        <v>4844319.4935910003</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>15.594155000000001</v>
+      </c>
+      <c r="E6">
+        <v>14.312487000000001</v>
+      </c>
+      <c r="F6">
+        <v>3.802686</v>
+      </c>
+      <c r="G6">
+        <v>10.193071</v>
+      </c>
+      <c r="H6">
+        <v>18.942261999999999</v>
+      </c>
+      <c r="I6">
+        <v>29.030825</v>
+      </c>
+      <c r="J6">
+        <v>38.522472999999998</v>
+      </c>
+      <c r="K6" s="1">
+        <v>527.56610799999999</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>14.729879</v>
+      </c>
+      <c r="E7">
+        <v>441.14876900000002</v>
+      </c>
+      <c r="F7">
+        <v>1619.73973</v>
+      </c>
+      <c r="G7">
+        <v>2488.3524710000002</v>
+      </c>
+      <c r="H7">
+        <v>6175.4351999999999</v>
+      </c>
+      <c r="I7">
+        <v>13254.281147</v>
+      </c>
+      <c r="J7">
+        <v>24521.592473000001</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1813793.797089</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D27BA5DC-5838-4C14-908D-A6BA561D683B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="F6:J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>